<commit_message>
solved few more question
</commit_message>
<xml_diff>
--- a/Road Map.xlsx
+++ b/Road Map.xlsx
@@ -3,22 +3,24 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20393"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F990ED9-BE65-40BC-BEDB-4DDC9D8DE31B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B476AB8-1A8D-44A3-B925-98A773E93947}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AIML" sheetId="1" r:id="rId1"/>
     <sheet name="React" sheetId="2" r:id="rId2"/>
     <sheet name="Leet Code QA" sheetId="10" r:id="rId3"/>
     <sheet name="System Design" sheetId="3" r:id="rId4"/>
-    <sheet name="Projects Repos" sheetId="8" r:id="rId5"/>
-    <sheet name="Interviews" sheetId="9" r:id="rId6"/>
-    <sheet name="DSA" sheetId="4" r:id="rId7"/>
-    <sheet name="Python" sheetId="5" r:id="rId8"/>
-    <sheet name="MS SQL" sheetId="6" r:id="rId9"/>
-    <sheet name="Excel" sheetId="7" r:id="rId10"/>
-    <sheet name="Full Stack" sheetId="11" r:id="rId11"/>
+    <sheet name="GIT" sheetId="12" r:id="rId5"/>
+    <sheet name="Useful Links" sheetId="13" r:id="rId6"/>
+    <sheet name="Projects Repos" sheetId="8" r:id="rId7"/>
+    <sheet name="Interviews" sheetId="9" r:id="rId8"/>
+    <sheet name="DSA" sheetId="4" r:id="rId9"/>
+    <sheet name="Python" sheetId="5" r:id="rId10"/>
+    <sheet name="MS SQL" sheetId="6" r:id="rId11"/>
+    <sheet name="Excel" sheetId="7" r:id="rId12"/>
+    <sheet name="Full Stack" sheetId="11" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="359">
   <si>
     <t>https://github.com/abhishekjdgsl/system-design-primer</t>
   </si>
@@ -1098,6 +1100,15 @@
   </si>
   <si>
     <t xml:space="preserve">System Design </t>
+  </si>
+  <si>
+    <t>https://learngitbranching.js.org/</t>
+  </si>
+  <si>
+    <t>For</t>
+  </si>
+  <si>
+    <t>GIT</t>
   </si>
 </sst>
 </file>
@@ -1693,6 +1704,144 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E755E76-A98E-4617-B381-1E9ABEE42EC5}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2" t="str">
+        <f>REPT("⭐", D2)</f>
+        <v>⭐⭐⭐</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC4824A9-78F8-4E13-98E1-09AA1C8B8653}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="27.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="86.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="str">
+        <f>REPT("⭐", D2)</f>
+        <v>⭐⭐</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="str">
+        <f>REPT("⭐", D3)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE0DB1CE-453E-46A5-A2A3-81F735C0FE59}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1706,7 +1855,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60416CE8-6F1D-44F6-8ED1-C0BE9B0B7C5C}">
   <dimension ref="C4:E4"/>
   <sheetViews>
@@ -3151,7 +3300,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{542BEBF3-7401-4FBF-B9E4-72C5EFA1BED8}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -3247,6 +3396,63 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5045F5-4EFD-453D-BE63-069069690CD1}">
+  <dimension ref="A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>356</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E587012A-0B12-4DF0-B2B8-529655519B34}">
+  <dimension ref="C4:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>356</v>
+      </c>
+      <c r="D5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5CFD591-6A71-4013-B915-2D45BA78B05D}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -3310,7 +3516,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB52F63E-91BE-4C21-8550-5B914499DE10}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -3372,7 +3578,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BFA6B71-11B8-4741-B793-7F901078DE7C}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -3488,142 +3694,4 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E755E76-A98E-4617-B381-1E9ABEE42EC5}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2" t="str">
-        <f>REPT("⭐", D2)</f>
-        <v>⭐⭐⭐</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC4824A9-78F8-4E13-98E1-09AA1C8B8653}">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="27.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="86.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2" t="str">
-        <f>REPT("⭐", D2)</f>
-        <v>⭐⭐</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" t="str">
-        <f>REPT("⭐", D3)</f>
-        <v/>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>